<commit_message>
Update sample TSV: add 4C to sample preservation temp (#575)
* Update sample TSV: add 4C to sample preservation temp

UFL uses 4C for sample preservation temp.

* Update src/ingest_validation_tools/table-schemas/sample.yaml

Co-authored-by: Nils Gehlenborg <nils@hms.harvard.edu>

* Update src/ingest_validation_tools/table-schemas/sample.yaml

* regen

* changelog

* Update error message in fixture

Co-authored-by: Nils Gehlenborg <nils@hms.harvard.edu>
Co-authored-by: Chuck McCallum <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/sample/sample.xlsx
+++ b/docs/sample/sample.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>sample_id</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Freezer (-20 Celsius)</t>
+  </si>
+  <si>
+    <t>Refrigerator (4 Celsius)</t>
   </si>
   <si>
     <t>Room Temperature</t>
@@ -721,13 +724,13 @@
         <v>23</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -758,8 +761,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: minutes." sqref="K2:K1048576">
       <formula1>'cold_ischemia_time_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Liquid Nitrogen / Liquid Nitrogen Vapor / Freezer (-80 Celsius) / Freezer (-20 Celsius) / Room Temperature." sqref="L2:L1048576">
-      <formula1>'specimen_prese...mperature list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from specimen_prese...mperature list." sqref="L2:L1048576">
+      <formula1>'specimen_prese...mperature list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="N2:N1048576">
       <formula1>-1e+307</formula1>
@@ -919,7 +922,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -948,6 +951,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +973,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sample metadata update: Add a new perfusion_solution (#666)
* sample metadata update: Add perfusion solution to enums

Add Belzer MPS/KPS to the dropdown for perfusion_solution.

* Regen

Co-authored-by: mccalluc <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/sample/sample.xlsx
+++ b/docs/sample/sample.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>sample_id</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>HTK</t>
+  </si>
+  <si>
+    <t>Belzer MPS/KPS</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -706,31 +709,31 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -744,8 +747,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: healthy / diseased." sqref="D2:D1048576">
       <formula1>'organ_condition list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: UWS / HTK / Unknown / None." sqref="F2:F1048576">
-      <formula1>'perfusion_solution list'!$A$1:$A$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: UWS / HTK / Belzer MPS/KPS / Unknown / None." sqref="F2:F1048576">
+      <formula1>'perfusion_solution list'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="H2:H1048576">
       <formula1>-1e+307</formula1>
@@ -853,7 +856,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -877,6 +880,11 @@
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +920,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -930,32 +938,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +981,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add formalin to enums for perfusion solutions (#695)
* Add formalin to perfusion solutions

GE uses formalin.

* Regen

Co-authored-by: mccalluc <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/sample/sample.xlsx
+++ b/docs/sample/sample.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>sample_id</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Belzer MPS/KPS</t>
+  </si>
+  <si>
+    <t>Formalin</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -709,31 +712,31 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +750,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: healthy / diseased." sqref="D2:D1048576">
       <formula1>'organ_condition list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: UWS / HTK / Belzer MPS/KPS / Unknown / None." sqref="F2:F1048576">
-      <formula1>'perfusion_solution list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from perfusion_solution list." sqref="F2:F1048576">
+      <formula1>'perfusion_solution list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="H2:H1048576">
       <formula1>-1e+307</formula1>
@@ -856,7 +859,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -885,6 +888,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -902,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -920,7 +928,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -938,32 +946,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -981,7 +989,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regen sample and organ
</commit_message>
<xml_diff>
--- a/docs/sample/sample.xlsx
+++ b/docs/sample/sample.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="vital_state list" sheetId="2" r:id="rId2"/>
-    <sheet name="health_status list" sheetId="3" r:id="rId3"/>
-    <sheet name="organ_condition list" sheetId="4" r:id="rId4"/>
-    <sheet name="perfusion_solution list" sheetId="5" r:id="rId5"/>
-    <sheet name="warm_ischemia_time_unit list" sheetId="6" r:id="rId6"/>
-    <sheet name="cold_ischemia_time_unit list" sheetId="7" r:id="rId7"/>
-    <sheet name="specimen_prese...mperature list" sheetId="8" r:id="rId8"/>
-    <sheet name="specimen_tumor...ance_unit list" sheetId="9" r:id="rId9"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="anatomical_region list" sheetId="3" r:id="rId3"/>
+    <sheet name="tissue list" sheetId="4" r:id="rId4"/>
+    <sheet name="weight_unit list" sheetId="5" r:id="rId5"/>
+    <sheet name="sample_tumor_distance_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="sample_preparation_media list" sheetId="7" r:id="rId7"/>
+    <sheet name="sample_prepara...mperature list" sheetId="8" r:id="rId8"/>
+    <sheet name="sample_storage_temperature list" sheetId="9" r:id="rId9"/>
+    <sheet name="notes list" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -36,7 +37,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>(No description for this field was supplied.)</t>
+          <t>Current version of schema.</t>
         </r>
       </text>
     </comment>
@@ -49,7 +50,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identify the vital state of the donor.</t>
+          <t>Unique identifier for the source (parent) from which the sample was taken.</t>
         </r>
       </text>
     </comment>
@@ -62,7 +63,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Patient's baseline physical condition prior to immediate event leading to organ/tissue acquisition. For example, if a relatively healthy patient suffers trauma, and as a result of reparative surgery, a tissue sample is collected, the subject will be deemed “relatively healthy”.   Likewise, a relatively healthy subject may have experienced trauma leading to brain death.  As a result of organ donation, a sample is collected.  In this scenario, the subject is deemed “relatively healthy.”</t>
+          <t>Unique identifier for the sample. Currently referred to as "tissue ID".</t>
         </r>
       </text>
     </comment>
@@ -75,7 +76,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Health status of the organ at the time of sample recovery.</t>
+          <t>Region within the organ.</t>
         </r>
       </text>
     </comment>
@@ -88,7 +89,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of procedure to procure organ.</t>
+          <t>Organ specific tissue.</t>
         </r>
       </text>
     </comment>
@@ -101,7 +102,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of solution that was used to perfuse the organ.</t>
+          <t>Sample weight.</t>
         </r>
       </text>
     </comment>
@@ -114,7 +115,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Further details on organ level QC checks.</t>
+          <t>Sample weight.</t>
         </r>
       </text>
     </comment>
@@ -127,7 +128,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time interval between cessation of blood flow and cooling to 4C.</t>
+          <t>If surgical sample, how far from the pathology was the sample obtained.</t>
         </r>
       </text>
     </comment>
@@ -140,7 +141,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time unit</t>
+          <t>Distance unit</t>
         </r>
       </text>
     </comment>
@@ -153,7 +154,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time interval on ice to the start of preservation protocol.</t>
+          <t>TODO</t>
         </r>
       </text>
     </comment>
@@ -166,7 +167,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time unit</t>
+          <t>What was the sample preserved in.</t>
         </r>
       </text>
     </comment>
@@ -179,7 +180,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature of the medium during the preservation process.</t>
+          <t>The temperature for the preparation process.</t>
         </r>
       </text>
     </comment>
@@ -192,7 +193,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>For example, RIN: 8.7.</t>
+          <t>The temperature during storage, after preparation and before the assay is performed.</t>
         </r>
       </text>
     </comment>
@@ -205,7 +206,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If surgical sample, how far from the tumor was the sample obtained from. Typically a number of centimeters. Leave blank if not applicable or unknown.</t>
+          <t>For example, RIN: 8.7</t>
         </r>
       </text>
     </comment>
@@ -218,7 +219,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Distance unit</t>
+          <t>Histopathological reporting of key variables that are important for the tissue (absence of necrosis, comment on composition, significant pathology description, high level inflammation/fibrosis assessment, etc.)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TODO</t>
         </r>
       </text>
     </comment>
@@ -227,87 +241,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
   <si>
     <t>sample_id</t>
   </si>
   <si>
-    <t>vital_state</t>
-  </si>
-  <si>
-    <t>living</t>
-  </si>
-  <si>
-    <t>deceased</t>
-  </si>
-  <si>
-    <t>health_status</t>
-  </si>
-  <si>
-    <t>cancer</t>
-  </si>
-  <si>
-    <t>relatively healthy</t>
-  </si>
-  <si>
-    <t>chronic illness</t>
-  </si>
-  <si>
-    <t>organ_condition</t>
-  </si>
-  <si>
-    <t>healthy</t>
-  </si>
-  <si>
-    <t>diseased</t>
-  </si>
-  <si>
-    <t>procedure_date</t>
-  </si>
-  <si>
-    <t>perfusion_solution</t>
-  </si>
-  <si>
-    <t>UWS</t>
-  </si>
-  <si>
-    <t>HTK</t>
-  </si>
-  <si>
-    <t>Belzer MPS/KPS</t>
-  </si>
-  <si>
-    <t>Formalin</t>
-  </si>
-  <si>
-    <t>Perfadex</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>pathologist_report</t>
-  </si>
-  <si>
-    <t>warm_ischemia_time_value</t>
-  </si>
-  <si>
-    <t>warm_ischemia_time_unit</t>
-  </si>
-  <si>
-    <t>minutes</t>
-  </si>
-  <si>
-    <t>cold_ischemia_time_value</t>
-  </si>
-  <si>
-    <t>cold_ischemia_time_unit</t>
-  </si>
-  <si>
-    <t>specimen_preservation_temperature</t>
+    <t>anatomical_region</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>weight_value</t>
+  </si>
+  <si>
+    <t>weight_unit</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>sample_pathology_distance_value</t>
+  </si>
+  <si>
+    <t>sample_tumor_distance_unit</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>sample_preparation_protocols_io_doi</t>
+  </si>
+  <si>
+    <t>sample_preparation_media</t>
+  </si>
+  <si>
+    <t>fresh</t>
+  </si>
+  <si>
+    <t>snap frozen</t>
+  </si>
+  <si>
+    <t>fresh frozen OCT</t>
+  </si>
+  <si>
+    <t>FFPE</t>
+  </si>
+  <si>
+    <t>RNAlater</t>
+  </si>
+  <si>
+    <t>4% PFA</t>
+  </si>
+  <si>
+    <t>fixed frozen OCT</t>
+  </si>
+  <si>
+    <t>Cellfreezing media</t>
+  </si>
+  <si>
+    <t>CMC</t>
+  </si>
+  <si>
+    <t>10% NBF</t>
+  </si>
+  <si>
+    <t>sample_preparation_temperature</t>
   </si>
   <si>
     <t>Liquid Nitrogen</t>
@@ -328,16 +339,22 @@
     <t>Room Temperature</t>
   </si>
   <si>
-    <t>specimen_quality_criteria</t>
-  </si>
-  <si>
-    <t>specimen_tumor_distance_value</t>
-  </si>
-  <si>
-    <t>specimen_tumor_distance_unit</t>
-  </si>
-  <si>
-    <t>cm</t>
+    <t>sample_storage_temperature</t>
+  </si>
+  <si>
+    <t>sample_quality_criteria</t>
+  </si>
+  <si>
+    <t>histological_report</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -686,7 +703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -695,90 +712,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: living / deceased." sqref="B2:B1048576">
-      <formula1>'vital_state list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: cancer / relatively healthy / chronic illness." sqref="C2:C1048576">
-      <formula1>'health_status list'!$A$1:$A$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TODO." sqref="D2:D1048576">
+      <formula1>'anatomical_region list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: healthy / diseased." sqref="D2:D1048576">
-      <formula1>'organ_condition list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TODO." sqref="E2:E1048576">
+      <formula1>'tissue list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from perfusion_solution list." sqref="F2:F1048576">
-      <formula1>'perfusion_solution list'!$A$1:$A$7</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="F2:F1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: g." sqref="G2:G1048576">
+      <formula1>'weight_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="H2:H1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: minutes." sqref="I2:I1048576">
-      <formula1>'warm_ischemia_time_unit list'!$A$1:$A$1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: cm." sqref="I2:I1048576">
+      <formula1>'sample_tumor_distance_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="J2:J1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from sample_preparation_media list." sqref="K2:K1048576">
+      <formula1>'sample_preparation_media list'!$A$1:$A$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: minutes." sqref="K2:K1048576">
-      <formula1>'cold_ischemia_time_unit list'!$A$1:$A$1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from sample_prepara...mperature list." sqref="L2:L1048576">
+      <formula1>'sample_prepara...mperature list'!$A$1:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from specimen_prese...mperature list." sqref="L2:L1048576">
-      <formula1>'specimen_prese...mperature list'!$A$1:$A$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from sample_storage_temperature list." sqref="M2:M1048576">
+      <formula1>'sample_storage_temperature list'!$A$1:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="N2:N1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: cm." sqref="O2:O1048576">
-      <formula1>'specimen_tumor...ance_unit list'!$A$1:$A$1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: left / right." sqref="P2:P1048576">
+      <formula1>'notes list'!$A$1:$A$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -786,7 +805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -796,12 +815,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -809,9 +828,27 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -822,16 +859,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -839,7 +866,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -848,59 +893,6 @@
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +920,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -936,7 +928,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -954,32 +991,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -997,7 +1034,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>